<commit_message>
All the excel generation codes are transferred into the Report app
</commit_message>
<xml_diff>
--- a/room_schedule_Computer_B-004.xlsx
+++ b/room_schedule_Computer_B-004.xlsx
@@ -14,7 +14,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="35">
+  <si>
+    <t>B-004</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>ES-IOTL</t>
+  </si>
+  <si>
+    <t>TEA</t>
+  </si>
+  <si>
+    <t>NSS</t>
+  </si>
+  <si>
+    <t>AAB</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>TEB</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>TEC</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
   <si>
     <t>Time</t>
   </si>
@@ -53,8 +125,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,12 +149,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF77ABFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -104,9 +202,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -403,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,153 +519,500 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="1" t="s">
+      <c r="D4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="1" t="s">
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="1"/>
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="1"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="1"/>
+      <c r="A34" s="3"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
-        <v>9</v>
+      <c r="A35" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="1"/>
+      <c r="A36" s="3"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="1"/>
+      <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="1"/>
+      <c r="A38" s="3"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="1" t="s">
-        <v>10</v>
+      <c r="A39" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="1"/>
+      <c r="A40" s="3"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="1"/>
+      <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="1"/>
+      <c r="A42" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="27">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A11:A14"/>

</xml_diff>